<commit_message>
add the final report format
</commit_message>
<xml_diff>
--- a/Report_format_2_complete.xlsx
+++ b/Report_format_2_complete.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Items to be improved</t>
   </si>
@@ -58,16 +58,7 @@
     <t>Xiaoliwan wax+Paste conductive foam+Lower glass glue frame dispensing operation saturation75%</t>
   </si>
   <si>
-    <t>The upper and lower glass bonding saturation is 67.5%</t>
-  </si>
-  <si>
-    <t>Five-in-one front&amp;back saturation53.2%</t>
-  </si>
-  <si>
-    <t>The improvement direction for 'The saturation of the lower glass point Xiaoli Pill is 65%' is: 1. Judgment of value and reduce tasks without added value 2. Inspection of movement quality and human engineering hazards: Reduce the number of movements, work with both hands at the same time, shorten the distance of movements, and make movements easier; eliminate human engineering hazards 3. Automated level inspection: simple and automated import 4. Merge and rearrange new job elements.</t>
-  </si>
-  <si>
-    <t>The 'Improvement direction' for 'Bottom glass electrophoresis tank+UVFixed baking operation saturation79.2%' is as follows: 1. Judgment of value and reduce tasks without added value 2. Inspection of movement quality and human engineering hazards: Reduce the number of movements, work with both hands at the same time, shorten the distance of movements, and make movements easier; eliminate human engineering hazards 3. Automated level inspection: simple and automated import 4. Merge and rearrange new job elements.</t>
+    <t>Low job saturation(lower than95%)</t>
   </si>
   <si>
     <t>1. Judgment of value and reduce tasks without added value
@@ -76,10 +67,13 @@
 4. Merge and rearrange new job elements</t>
   </si>
   <si>
-    <t>The improvement direction for 'The upper and lower glass bonding saturation is 67.5%' is as follows: 1. Judgment of value and reduce tasks without added value 2. Inspection of movement quality and human engineering hazards: Reduce the number of movements, work with both hands at the same time, shorten the distance of movements, and make movements easier; eliminate human engineering hazards 3. Automated level inspection: simple and automated import 4. Merge and rearrange new job elements.</t>
-  </si>
-  <si>
-    <t>The 'Improvement direction' for 'Five-in-one front&amp;back saturation53.2%' is to reduce the number of movements, work with both hands at the same time, shorten the distance of movements, and make movements easier; eliminate human engineering hazards.</t>
+    <t>The improvement direction for the problem 'Bottom glass electrophoresis tank+UVFixed baking operation saturation79.2%' is as follows: 1. Judgment of value and reduce tasks without added value 2. Inspection of movement quality and human engineering hazards: Reduce the number of movements, work with both hands at the same time, shorten the distance of movements, and make movements easier; eliminate human engineering hazards 3. Automated level inspection: simple and automated import 4. Merge and rearrange new job elements.</t>
+  </si>
+  <si>
+    <t>1. Judgment of value and reduce tasks without added value
+2. Inspection of movement quality and human engineering hazards
+3. Automated level inspection
+4. Merge and rearrange new job elements</t>
   </si>
   <si>
     <t>LiXX</t>
@@ -91,7 +85,16 @@
     <t>10/15/24</t>
   </si>
   <si>
+    <t>Expected completion date: 10/15/24</t>
+  </si>
+  <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>The improvement parameter 'Confirmation' for the problem 'Bottom glass electrophoresis tank+UVFixed baking operation saturation79.2%' is 'yes'.</t>
+  </si>
+  <si>
+    <t>The improvement parameter 'Confirmation' for the problem 'Xiaoliwan wax+Paste conductive foam+Lower glass glue frame dispensing operation saturation75%' is 'yes'.</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,148 +497,105 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>12</v>
       </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
       <c r="K3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
       <c r="K4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>